<commit_message>
implementando lista de DataType
</commit_message>
<xml_diff>
--- a/dist/dados-com-template.xlsx
+++ b/dist/dados-com-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHome\ws-github\csvintoexcel\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099FD8A0-ACF1-41D1-8BD0-112933B5BCF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FFAD07-B41B-41BD-8B7A-254213FA0A6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{61C264D4-E676-4BA5-A77A-185EE75A4B25}"/>
   </bookViews>
@@ -30,169 +30,192 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
   <si>
     <t>Josemar Silva</t>
   </si>
   <si>
+    <t>Col-A(Int)</t>
+  </si>
+  <si>
+    <t>Col-B(Double)</t>
+  </si>
+  <si>
+    <t>Col-C(Date)</t>
+  </si>
+  <si>
+    <t>Col-D(Text)</t>
+  </si>
+  <si>
+    <t>Col-E(Date-fmt)</t>
+  </si>
+  <si>
+    <t>Col-F(Double-fmt)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1,01</t>
+  </si>
+  <si>
+    <t>25/04/1969</t>
+  </si>
+  <si>
+    <t>123456789012345</t>
+  </si>
+  <si>
+    <t>3,14159</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2,02</t>
+  </si>
+  <si>
+    <t>25/10/2004</t>
+  </si>
+  <si>
+    <t>6,28319</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>3,03</t>
+  </si>
+  <si>
+    <t>21/07/1938</t>
+  </si>
+  <si>
     <t>Maria do Carmo</t>
   </si>
   <si>
+    <t>9,42478</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>4,04</t>
+  </si>
+  <si>
+    <t>15/10/1972</t>
+  </si>
+  <si>
     <t>Maria Stela</t>
   </si>
   <si>
+    <t>12,56637</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>5,05</t>
+  </si>
+  <si>
+    <t>22/01/1993</t>
+  </si>
+  <si>
     <t>Guilherme</t>
   </si>
   <si>
+    <t>15,70796</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>6,06</t>
+  </si>
+  <si>
+    <t>15/08/2001</t>
+  </si>
+  <si>
     <t>Gabriele</t>
   </si>
   <si>
+    <t>18,84956</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>7,07</t>
+  </si>
+  <si>
     <t>Antonio</t>
   </si>
   <si>
+    <t>21,99115</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>8,08</t>
+  </si>
+  <si>
     <t>Pedro</t>
   </si>
   <si>
+    <t>25,13274</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>9,09</t>
+  </si>
+  <si>
     <t>Paulo</t>
   </si>
   <si>
+    <t>28,27433</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10,1</t>
+  </si>
+  <si>
     <t>José</t>
   </si>
   <si>
-    <t>Col-A(Int)</t>
-  </si>
-  <si>
-    <t>Col-B(Double)</t>
-  </si>
-  <si>
-    <t>Col-C(Date)</t>
-  </si>
-  <si>
-    <t>Col-D(Text)</t>
-  </si>
-  <si>
-    <t>Col-E(Date-fmt)</t>
-  </si>
-  <si>
-    <t>Col-F(Double-fmt)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>25/04/1969</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>2,02</t>
-  </si>
-  <si>
-    <t>25/10/2004</t>
-  </si>
-  <si>
-    <t>6,28319</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>3,03</t>
-  </si>
-  <si>
-    <t>21/07/1938</t>
-  </si>
-  <si>
-    <t>9,42478</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>4,04</t>
-  </si>
-  <si>
-    <t>15/10/1972</t>
-  </si>
-  <si>
-    <t>12,56637</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>5,05</t>
-  </si>
-  <si>
-    <t>22/01/1993</t>
-  </si>
-  <si>
-    <t>15,70796</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>6,06</t>
-  </si>
-  <si>
-    <t>15/08/2001</t>
-  </si>
-  <si>
-    <t>18,84956</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>7,07</t>
-  </si>
-  <si>
-    <t>21,99115</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>8,08</t>
-  </si>
-  <si>
-    <t>25,13274</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>9,09</t>
-  </si>
-  <si>
-    <t>28,27433</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>10,1</t>
-  </si>
-  <si>
     <t>31,41593</t>
   </si>
   <si>
-    <t>JosÃ©</t>
+    <t>11</t>
+  </si>
+  <si>
+    <t>11,1</t>
+  </si>
+  <si>
+    <t>27/10/1985</t>
+  </si>
+  <si>
+    <t>Alex Barbosa</t>
+  </si>
+  <si>
+    <t>33,333333</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0_ ;\-0\ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +225,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -241,18 +271,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,243 +597,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F90794C-5C2F-416A-AE61-3811430F8DE1}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.28515625" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="35.28515625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1" t="str">
-        <f>A2/100+A2</f>
-        <v>1,01</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1.01</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="str">
-        <f>C2</f>
-        <v>25/04/1969</v>
-      </c>
-      <c r="F2" s="3" t="str">
-        <f t="shared" ref="F2:F10" si="0">PI()*(ROW()-1)</f>
-        <v>3,14159</v>
+      <c r="E2" s="5" t="n">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>3.14159</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="1">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s" s="1">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B3" t="n" s="1">
+        <v>2.02</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="E3" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s" s="3">
-        <v>21</v>
+      <c r="E3" t="n" s="5">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F3" t="n" s="3">
+        <v>6.28319</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="1">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s" s="1">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="B4" t="n" s="1">
+        <v>3.03</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s" s="3">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="E4" t="n" s="5">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F4" t="n" s="3">
+        <v>9.42478</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s" s="1">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="B5" t="n" s="1">
+        <v>4.04</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s" s="1">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s" s="3">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="E5" t="n" s="5">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F5" t="n" s="3">
+        <v>12.56637</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="B6" t="n" s="1">
+        <v>5.05</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s" s="1">
         <v>30</v>
       </c>
-      <c r="B6" t="s" s="1">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s" s="1">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s" s="3">
-        <v>33</v>
+      <c r="E6" t="n" s="5">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F6" t="n" s="3">
+        <v>15.70796</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="B7" t="n" s="1">
+        <v>6.06</v>
+      </c>
+      <c r="C7" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="B7" t="s" s="1">
+      <c r="D7" t="s" s="1">
         <v>35</v>
       </c>
-      <c r="C7" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s" s="1">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s" s="3">
-        <v>37</v>
+      <c r="E7" t="n" s="5">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F7" t="n" s="3">
+        <v>18.84956</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="B8" t="n" s="1">
+        <v>7.07</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s" s="1">
         <v>39</v>
       </c>
-      <c r="C8" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s" s="3">
-        <v>40</v>
+      <c r="E8" t="n" s="5">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F8" t="n" s="3">
+        <v>21.99115</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
         <v>41</v>
       </c>
-      <c r="B9" t="s" s="1">
-        <v>42</v>
+      <c r="B9" t="n" s="1">
+        <v>8.08</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s" s="1">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s" s="3">
         <v>43</v>
+      </c>
+      <c r="E9" t="n" s="5">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F9" t="n" s="3">
+        <v>25.13274</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s" s="1">
         <v>45</v>
       </c>
+      <c r="B10" t="n" s="1">
+        <v>9.09</v>
+      </c>
       <c r="C10" t="s" s="2">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s" s="1">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s" s="3">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="E10" t="n" s="5">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F10" t="n" s="3">
+        <v>28.27433</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s" s="1">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="B11" t="n" s="1">
+        <v>10.1</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s" s="1">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s" s="3">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="E11" t="n" s="5">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F11" t="n" s="3">
+        <v>31.41593</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="1">
+        <v>53</v>
+      </c>
+      <c r="B12" t="n" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s" s="1">
+        <v>56</v>
+      </c>
+      <c r="E12" t="n" s="5">
+        <v>1.23456789012345E14</v>
+      </c>
+      <c r="F12" t="n" s="3">
+        <v>33.333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>